<commit_message>
Add averages to results spreadsheet
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jav26\Documents\MEGAsync\School\Parallel-21\ParallelProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2562F265-51CA-4FBB-B45A-3EF684D008D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52695E31-6D7F-41CA-8E33-4FBF2480466C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="5730" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{046285F4-ADCD-4FEF-A095-5EC34F5654E5}"/>
+    <workbookView xWindow="-25320" yWindow="5730" windowWidth="25440" windowHeight="15390" xr2:uid="{046285F4-ADCD-4FEF-A095-5EC34F5654E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Python" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="7">
   <si>
     <t>Processor Count</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>15 decimal precision</t>
+  </si>
+  <si>
+    <t>avg</t>
   </si>
 </sst>
 </file>
@@ -265,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -304,6 +307,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4433,16 +4437,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>202925</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>177248</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>422000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>110573</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>484533</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>178905</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>94008</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>112230</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4898,8 +4902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E19EC56-D95B-418F-A39D-3BAEC706A45A}">
   <dimension ref="A3:H27"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5118,7 +5122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="4">
         <v>2</v>
@@ -5144,7 +5148,7 @@
         <v>1.936626064354303</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="4">
         <v>4</v>
@@ -5169,8 +5173,11 @@
         <f t="shared" si="1"/>
         <v>3.279813331549907</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21"/>
       <c r="B19" s="8">
         <v>8</v>
@@ -5195,9 +5202,13 @@
         <f>G7/G10</f>
         <v>4.8504134637923135</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="H19" s="22">
+        <f>AVERAGE(C19:G19)</f>
+        <v>3.0849767364532896</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="14" t="s">
         <v>3</v>
@@ -5208,7 +5219,7 @@
       <c r="F21" s="14"/>
       <c r="G21" s="15"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="1"/>
       <c r="C22" s="16" t="s">
@@ -5219,7 +5230,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="18"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="4" t="s">
         <v>5</v>
@@ -5240,7 +5251,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>0</v>
       </c>
@@ -5268,7 +5279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
       <c r="B25" s="4">
         <v>2</v>
@@ -5294,7 +5305,7 @@
         <v>0.96831303217715148</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
       <c r="B26" s="4">
         <v>4</v>
@@ -5320,7 +5331,7 @@
         <v>0.81995333288747674</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="21"/>
       <c r="B27" s="8">
         <v>8</v>
@@ -5368,8 +5379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F52FEB7-AA35-469B-ACB7-E2AA330F9581}">
   <dimension ref="A3:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5588,7 +5599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="4">
         <v>2</v>
@@ -5614,7 +5625,7 @@
         <v>1.9521823655409603</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="4">
         <v>4</v>
@@ -5639,8 +5650,11 @@
         <f t="shared" si="1"/>
         <v>3.8478554505792957</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21"/>
       <c r="B19" s="8">
         <v>8</v>
@@ -5665,9 +5679,13 @@
         <f>G7/G10</f>
         <v>7.6721034060632256</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="H19" s="22">
+        <f>AVERAGE(C19:G19)</f>
+        <v>7.5887950718247339</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="14" t="s">
         <v>3</v>
@@ -5678,7 +5696,7 @@
       <c r="F21" s="14"/>
       <c r="G21" s="15"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="1"/>
       <c r="C22" s="16" t="s">
@@ -5689,7 +5707,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="18"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="4" t="s">
         <v>5</v>
@@ -5710,7 +5728,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>0</v>
       </c>
@@ -5738,7 +5756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
       <c r="B25" s="4">
         <v>2</v>
@@ -5764,7 +5782,7 @@
         <v>0.97609118277048013</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
       <c r="B26" s="4">
         <v>4</v>
@@ -5790,7 +5808,7 @@
         <v>0.96196386264482392</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="21"/>
       <c r="B27" s="8">
         <v>8</v>
@@ -5839,7 +5857,7 @@
   <dimension ref="A3:H27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6058,7 +6076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="4">
         <v>2</v>
@@ -6084,7 +6102,7 @@
         <v>2.0018709344720582</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="4">
         <v>4</v>
@@ -6109,8 +6127,11 @@
         <f t="shared" si="1"/>
         <v>3.9426262223109161</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21"/>
       <c r="B19" s="8">
         <v>8</v>
@@ -6135,9 +6156,13 @@
         <f>G7/G10</f>
         <v>6.9608471067880533</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="H19" s="22">
+        <f>AVERAGE(C19:G19)</f>
+        <v>4.6424402631084574</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="14" t="s">
         <v>3</v>
@@ -6148,7 +6173,7 @@
       <c r="F21" s="14"/>
       <c r="G21" s="15"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="1"/>
       <c r="C22" s="16" t="s">
@@ -6159,7 +6184,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="18"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="4" t="s">
         <v>5</v>
@@ -6180,7 +6205,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>0</v>
       </c>
@@ -6208,7 +6233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
       <c r="B25" s="4">
         <v>2</v>
@@ -6234,7 +6259,7 @@
         <v>1.0009354672360291</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
       <c r="B26" s="4">
         <v>4</v>
@@ -6260,7 +6285,7 @@
         <v>0.98565655557772902</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="21"/>
       <c r="B27" s="8">
         <v>8</v>
@@ -6309,7 +6334,7 @@
   <dimension ref="A3:H27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6528,7 +6553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="4">
         <v>2</v>
@@ -6554,7 +6579,7 @@
         <v>1.8256133031010473</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="4">
         <v>4</v>
@@ -6579,8 +6604,11 @@
         <f t="shared" si="1"/>
         <v>3.6747926555294677</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21"/>
       <c r="B19" s="8">
         <v>8</v>
@@ -6605,9 +6633,13 @@
         <f>G7/G10</f>
         <v>7.5042565814890452</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="H19" s="22">
+        <f>AVERAGE(C19:G19)</f>
+        <v>5.9630586710983193</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="14" t="s">
         <v>3</v>
@@ -6618,7 +6650,7 @@
       <c r="F21" s="14"/>
       <c r="G21" s="15"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="1"/>
       <c r="C22" s="16" t="s">
@@ -6629,7 +6661,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="18"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="4" t="s">
         <v>5</v>
@@ -6650,7 +6682,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>0</v>
       </c>
@@ -6678,7 +6710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
       <c r="B25" s="4">
         <v>2</v>
@@ -6704,7 +6736,7 @@
         <v>0.91280665155052365</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
       <c r="B26" s="4">
         <v>4</v>
@@ -6730,7 +6762,7 @@
         <v>0.91869816388236691</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="21"/>
       <c r="B27" s="8">
         <v>8</v>

</xml_diff>